<commit_message>
Updated all document formats for that semester with exercise 3,4 and 5 task 1 and 2
</commit_message>
<xml_diff>
--- a/2_Semester/aufgabe_3+4+5_team_3_lernjournal.xlsx
+++ b/2_Semester/aufgabe_3+4+5_team_3_lernjournal.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="38140" yWindow="1800" windowWidth="27120" windowHeight="18980" tabRatio="415" activeTab="2"/>
+    <workbookView xWindow="36740" yWindow="1520" windowWidth="30420" windowHeight="18620" tabRatio="415" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Lernjournal Aufgabe 3" sheetId="3" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="56">
   <si>
     <t>Anleitung zum Lernjournal:</t>
   </si>
@@ -203,6 +203,15 @@
   </si>
   <si>
     <t>Besprechung Aufgabenstellung 2+3 und Analyse der gevorderten Lösungen</t>
+  </si>
+  <si>
+    <t>Diagramm(e) zm drei Schichten Modell überarbeitet mit Factory und Singleton / Abstrakter Klasse - Interface ergänzt.</t>
+  </si>
+  <si>
+    <t>7.12.13</t>
+  </si>
+  <si>
+    <t>1.12.13</t>
   </si>
 </sst>
 </file>
@@ -401,7 +410,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="125">
+  <cellStyleXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -527,8 +536,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
@@ -683,11 +696,14 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="125">
+  <cellStyles count="129">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -750,6 +766,8 @@
     <cellStyle name="Besuchter Link" xfId="120" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="122" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="128" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -812,6 +830,8 @@
     <cellStyle name="Link" xfId="119" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="121" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="127" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1174,11 +1194,11 @@
       <c r="P1" s="2"/>
     </row>
     <row r="2" spans="1:16" s="4" customFormat="1" ht="60" customHeight="1">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -2438,11 +2458,11 @@
       <c r="P1" s="2"/>
     </row>
     <row r="2" spans="1:16" s="4" customFormat="1" ht="60" customHeight="1">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -3534,7 +3554,7 @@
   <dimension ref="A1:P42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="A13" sqref="A13:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -3564,11 +3584,11 @@
       <c r="P1" s="2"/>
     </row>
     <row r="2" spans="1:16" s="4" customFormat="1" ht="60" customHeight="1">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -3763,14 +3783,16 @@
       <c r="O11" s="10"/>
       <c r="P11" s="10"/>
     </row>
-    <row r="12" spans="1:16" s="11" customFormat="1">
-      <c r="A12" s="8" t="s">
+    <row r="12" spans="1:16" s="11" customFormat="1" ht="13" thickBot="1">
+      <c r="A12" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="31">
         <v>20</v>
       </c>
-      <c r="C12" s="9"/>
+      <c r="C12" s="32" t="s">
+        <v>55</v>
+      </c>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
@@ -3785,10 +3807,16 @@
       <c r="O12" s="10"/>
       <c r="P12" s="10"/>
     </row>
-    <row r="13" spans="1:16" s="11" customFormat="1">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="9"/>
+    <row r="13" spans="1:16" s="11" customFormat="1" ht="25" thickTop="1">
+      <c r="A13" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="44">
+        <v>90</v>
+      </c>
+      <c r="C13" s="52" t="s">
+        <v>54</v>
+      </c>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
@@ -3845,7 +3873,7 @@
       </c>
       <c r="B16" s="18">
         <f>SUM(B11:B15)</f>
-        <v>80</v>
+        <v>170</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="2"/>
@@ -4004,14 +4032,14 @@
       <c r="O23" s="10"/>
       <c r="P23" s="10"/>
     </row>
-    <row r="24" spans="1:16" s="11" customFormat="1">
-      <c r="A24" s="23" t="s">
+    <row r="24" spans="1:16" s="11" customFormat="1" ht="13" thickBot="1">
+      <c r="A24" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="23">
+      <c r="B24" s="31">
         <v>35</v>
       </c>
-      <c r="C24" s="24" t="s">
+      <c r="C24" s="32" t="s">
         <v>38</v>
       </c>
       <c r="D24" s="10"/>
@@ -4028,10 +4056,16 @@
       <c r="O24" s="10"/>
       <c r="P24" s="10"/>
     </row>
-    <row r="25" spans="1:16" s="11" customFormat="1">
-      <c r="A25" s="23"/>
-      <c r="B25" s="23"/>
-      <c r="C25" s="24"/>
+    <row r="25" spans="1:16" s="11" customFormat="1" ht="25" thickTop="1">
+      <c r="A25" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" s="44">
+        <v>90</v>
+      </c>
+      <c r="C25" s="52" t="s">
+        <v>54</v>
+      </c>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
       <c r="F25" s="10"/>
@@ -4124,7 +4158,7 @@
       </c>
       <c r="B30" s="18">
         <f>SUM(B23:B29)</f>
-        <v>95</v>
+        <v>185</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="2"/>
@@ -4354,11 +4388,11 @@
       </c>
       <c r="B42" s="16">
         <f>SUM(B30,B16)</f>
-        <v>175</v>
+        <v>355</v>
       </c>
       <c r="C42" s="17">
         <f>TIME(0,B42,)</f>
-        <v>0.12152777777777778</v>
+        <v>0.24652777777777779</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>

</xml_diff>

<commit_message>
Lernjournal Aufgabe 5 Teil 3-5
</commit_message>
<xml_diff>
--- a/2_Semester/aufgabe_3+4+5_team_3_lernjournal.xlsx
+++ b/2_Semester/aufgabe_3+4+5_team_3_lernjournal.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="36740" yWindow="1520" windowWidth="30420" windowHeight="18620" tabRatio="415" activeTab="2"/>
+    <workbookView xWindow="36735" yWindow="1515" windowWidth="20730" windowHeight="11760" tabRatio="415" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Lernjournal Aufgabe 3" sheetId="3" r:id="rId1"/>
     <sheet name="Lernjournal Aufgabe 4" sheetId="2" r:id="rId2"/>
     <sheet name="Lernjournal Aufgabe 5" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="60">
   <si>
     <t>Anleitung zum Lernjournal:</t>
   </si>
@@ -213,16 +213,30 @@
   <si>
     <t>1.12.13</t>
   </si>
+  <si>
+    <t>Sequenzdiagramm 1.Version/Vorschlag</t>
+  </si>
+  <si>
+    <t>Vorbereitung Unterlagen studieren Sequenzdiagramm</t>
+  </si>
+  <si>
+    <t>Besprechung und Endversion Sequenzdiagramm. 
+Übernahme der Erkenntisse ins Klassendiagramm</t>
+  </si>
+  <si>
+    <t>Besprechung und Endversion Sequenzdiagramm. _x000D_
+Übernahme der Erkenntisse ins Klassendiagramm</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="???\ &quot;Minuten&quot;"/>
     <numFmt numFmtId="165" formatCode="[hh]:mm\ &quot;Std:Min&quot;"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -541,7 +555,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
@@ -702,136 +716,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="129">
-    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="92" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="94" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="96" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="98" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="100" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="102" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="104" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="106" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="108" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="110" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="112" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="114" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="116" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="118" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="120" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="122" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="124" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="126" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="128" builtinId="9" hidden="1"/>
-    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="69" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="71" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="73" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="75" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="77" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="79" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="81" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="83" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="85" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="87" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="89" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="91" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="93" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="95" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="97" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="99" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="101" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="103" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="105" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="107" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="109" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="111" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="113" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="115" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="117" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="119" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="121" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="123" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="125" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1160,20 +1180,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P57"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="68.1640625" customWidth="1"/>
-    <col min="2" max="3" width="12.1640625" customWidth="1"/>
+    <col min="1" max="1" width="68.140625" customWidth="1"/>
+    <col min="2" max="3" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="4" customFormat="1" ht="15">
+    <row r="1" spans="1:16" s="4" customFormat="1" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1249,7 +1269,7 @@
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
     </row>
-    <row r="5" spans="1:16" s="4" customFormat="1" ht="15">
+    <row r="5" spans="1:16" s="4" customFormat="1" ht="15.75">
       <c r="A5" s="5" t="s">
         <v>13</v>
       </c>
@@ -1305,7 +1325,7 @@
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
     </row>
-    <row r="8" spans="1:16" s="4" customFormat="1" ht="15">
+    <row r="8" spans="1:16" s="4" customFormat="1" ht="15.75">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -1345,7 +1365,7 @@
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
     </row>
-    <row r="10" spans="1:16" s="4" customFormat="1">
+    <row r="10" spans="1:16" s="4" customFormat="1" ht="25.5">
       <c r="A10" s="6" t="s">
         <v>4</v>
       </c>
@@ -1465,7 +1485,7 @@
       <c r="O14" s="10"/>
       <c r="P14" s="10"/>
     </row>
-    <row r="15" spans="1:16" s="11" customFormat="1" ht="37" thickBot="1">
+    <row r="15" spans="1:16" s="11" customFormat="1" ht="39" thickBot="1">
       <c r="A15" s="30" t="s">
         <v>19</v>
       </c>
@@ -1489,7 +1509,7 @@
       <c r="O15" s="10"/>
       <c r="P15" s="10"/>
     </row>
-    <row r="16" spans="1:16" s="11" customFormat="1" ht="13" thickTop="1">
+    <row r="16" spans="1:16" s="11" customFormat="1" ht="13.5" thickTop="1">
       <c r="A16" s="33" t="s">
         <v>24</v>
       </c>
@@ -1561,7 +1581,7 @@
       <c r="O18" s="10"/>
       <c r="P18" s="10"/>
     </row>
-    <row r="19" spans="1:16" s="11" customFormat="1" ht="25" thickBot="1">
+    <row r="19" spans="1:16" s="11" customFormat="1" ht="26.25" thickBot="1">
       <c r="A19" s="36" t="s">
         <v>28</v>
       </c>
@@ -1585,7 +1605,7 @@
       <c r="O19" s="10"/>
       <c r="P19" s="10"/>
     </row>
-    <row r="20" spans="1:16" s="11" customFormat="1" ht="13" thickTop="1">
+    <row r="20" spans="1:16" s="11" customFormat="1" ht="13.5" thickTop="1">
       <c r="A20" s="39" t="s">
         <v>29</v>
       </c>
@@ -1749,7 +1769,7 @@
       <c r="O27" s="2"/>
       <c r="P27" s="2"/>
     </row>
-    <row r="28" spans="1:16" s="4" customFormat="1" ht="15">
+    <row r="28" spans="1:16" s="4" customFormat="1" ht="15.75">
       <c r="A28" s="5" t="s">
         <v>9</v>
       </c>
@@ -1789,7 +1809,7 @@
       <c r="O29" s="2"/>
       <c r="P29" s="2"/>
     </row>
-    <row r="30" spans="1:16" s="4" customFormat="1">
+    <row r="30" spans="1:16" s="4" customFormat="1" ht="25.5">
       <c r="A30" s="6" t="s">
         <v>4</v>
       </c>
@@ -1813,7 +1833,7 @@
       <c r="O30" s="2"/>
       <c r="P30" s="2"/>
     </row>
-    <row r="31" spans="1:16" s="11" customFormat="1">
+    <row r="31" spans="1:16" s="11" customFormat="1" ht="25.5">
       <c r="A31" s="29" t="s">
         <v>20</v>
       </c>
@@ -1861,7 +1881,7 @@
       <c r="O32" s="10"/>
       <c r="P32" s="10"/>
     </row>
-    <row r="33" spans="1:16" s="11" customFormat="1">
+    <row r="33" spans="1:16" s="11" customFormat="1" ht="25.5">
       <c r="A33" s="23" t="s">
         <v>22</v>
       </c>
@@ -1909,7 +1929,7 @@
       <c r="O34" s="10"/>
       <c r="P34" s="10"/>
     </row>
-    <row r="35" spans="1:16" s="11" customFormat="1" ht="37" thickBot="1">
+    <row r="35" spans="1:16" s="11" customFormat="1" ht="39" thickBot="1">
       <c r="A35" s="30" t="s">
         <v>19</v>
       </c>
@@ -1933,7 +1953,7 @@
       <c r="O35" s="10"/>
       <c r="P35" s="10"/>
     </row>
-    <row r="36" spans="1:16" s="11" customFormat="1" ht="25" thickTop="1">
+    <row r="36" spans="1:16" s="11" customFormat="1" ht="39" thickTop="1">
       <c r="A36" s="33" t="s">
         <v>14</v>
       </c>
@@ -2053,7 +2073,7 @@
       <c r="O40" s="10"/>
       <c r="P40" s="10"/>
     </row>
-    <row r="41" spans="1:16" s="11" customFormat="1" ht="25" thickBot="1">
+    <row r="41" spans="1:16" s="11" customFormat="1" ht="26.25" thickBot="1">
       <c r="A41" s="36" t="s">
         <v>28</v>
       </c>
@@ -2077,7 +2097,7 @@
       <c r="O41" s="10"/>
       <c r="P41" s="10"/>
     </row>
-    <row r="42" spans="1:16" s="11" customFormat="1" ht="13" thickTop="1">
+    <row r="42" spans="1:16" s="11" customFormat="1" ht="13.5" thickTop="1">
       <c r="A42" s="25" t="s">
         <v>30</v>
       </c>
@@ -2223,7 +2243,7 @@
       <c r="O48" s="2"/>
       <c r="P48" s="2"/>
     </row>
-    <row r="49" spans="1:16" s="4" customFormat="1" ht="15" hidden="1">
+    <row r="49" spans="1:16" s="4" customFormat="1" ht="15.75" hidden="1">
       <c r="A49" s="5" t="s">
         <v>2</v>
       </c>
@@ -2263,7 +2283,7 @@
       <c r="O50" s="2"/>
       <c r="P50" s="2"/>
     </row>
-    <row r="51" spans="1:16" s="4" customFormat="1" hidden="1">
+    <row r="51" spans="1:16" s="4" customFormat="1" ht="25.5" hidden="1">
       <c r="A51" s="6" t="s">
         <v>4</v>
       </c>
@@ -2376,7 +2396,7 @@
       <c r="O55" s="2"/>
       <c r="P55" s="2"/>
     </row>
-    <row r="57" spans="1:16" s="4" customFormat="1" ht="17" customHeight="1">
+    <row r="57" spans="1:16" s="4" customFormat="1" ht="17.100000000000001" customHeight="1">
       <c r="A57" s="15" t="s">
         <v>11</v>
       </c>
@@ -2424,20 +2444,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P53"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="68.1640625" customWidth="1"/>
-    <col min="2" max="3" width="12.1640625" customWidth="1"/>
+    <col min="1" max="1" width="68.140625" customWidth="1"/>
+    <col min="2" max="3" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="4" customFormat="1" ht="15">
+    <row r="1" spans="1:16" s="4" customFormat="1" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2513,7 +2533,7 @@
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
     </row>
-    <row r="5" spans="1:16" s="4" customFormat="1" ht="15">
+    <row r="5" spans="1:16" s="4" customFormat="1" ht="15.75">
       <c r="A5" s="5" t="s">
         <v>13</v>
       </c>
@@ -2569,7 +2589,7 @@
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
     </row>
-    <row r="8" spans="1:16" s="4" customFormat="1" ht="15">
+    <row r="8" spans="1:16" s="4" customFormat="1" ht="15.75">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -2609,7 +2629,7 @@
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
     </row>
-    <row r="10" spans="1:16" s="4" customFormat="1">
+    <row r="10" spans="1:16" s="4" customFormat="1" ht="25.5">
       <c r="A10" s="6" t="s">
         <v>4</v>
       </c>
@@ -2657,7 +2677,7 @@
       <c r="O11" s="10"/>
       <c r="P11" s="10"/>
     </row>
-    <row r="12" spans="1:16" s="11" customFormat="1" ht="13" thickBot="1">
+    <row r="12" spans="1:16" s="11" customFormat="1" ht="13.5" thickBot="1">
       <c r="A12" s="30" t="s">
         <v>39</v>
       </c>
@@ -2681,7 +2701,7 @@
       <c r="O12" s="10"/>
       <c r="P12" s="10"/>
     </row>
-    <row r="13" spans="1:16" s="11" customFormat="1" ht="13" thickTop="1">
+    <row r="13" spans="1:16" s="11" customFormat="1" ht="13.5" thickTop="1">
       <c r="A13" s="44"/>
       <c r="B13" s="34"/>
       <c r="C13" s="35"/>
@@ -2699,7 +2719,7 @@
       <c r="O13" s="10"/>
       <c r="P13" s="10"/>
     </row>
-    <row r="14" spans="1:16" s="11" customFormat="1" ht="24">
+    <row r="14" spans="1:16" s="11" customFormat="1" ht="25.5">
       <c r="A14" s="20" t="s">
         <v>44</v>
       </c>
@@ -2723,7 +2743,7 @@
       <c r="O14" s="10"/>
       <c r="P14" s="10"/>
     </row>
-    <row r="15" spans="1:16" s="11" customFormat="1" ht="24">
+    <row r="15" spans="1:16" s="11" customFormat="1" ht="25.5">
       <c r="A15" s="25" t="s">
         <v>49</v>
       </c>
@@ -2917,7 +2937,7 @@
       <c r="O24" s="2"/>
       <c r="P24" s="2"/>
     </row>
-    <row r="25" spans="1:16" s="4" customFormat="1" ht="15">
+    <row r="25" spans="1:16" s="4" customFormat="1" ht="15.75">
       <c r="A25" s="5" t="s">
         <v>9</v>
       </c>
@@ -2957,7 +2977,7 @@
       <c r="O26" s="2"/>
       <c r="P26" s="2"/>
     </row>
-    <row r="27" spans="1:16" s="4" customFormat="1">
+    <row r="27" spans="1:16" s="4" customFormat="1" ht="25.5">
       <c r="A27" s="6" t="s">
         <v>4</v>
       </c>
@@ -3005,7 +3025,7 @@
       <c r="O28" s="10"/>
       <c r="P28" s="10"/>
     </row>
-    <row r="29" spans="1:16" s="11" customFormat="1" ht="24">
+    <row r="29" spans="1:16" s="11" customFormat="1" ht="25.5">
       <c r="A29" s="23" t="s">
         <v>33</v>
       </c>
@@ -3077,7 +3097,7 @@
       <c r="O31" s="10"/>
       <c r="P31" s="10"/>
     </row>
-    <row r="32" spans="1:16" s="11" customFormat="1" ht="13" thickBot="1">
+    <row r="32" spans="1:16" s="11" customFormat="1" ht="13.5" thickBot="1">
       <c r="A32" s="30" t="s">
         <v>39</v>
       </c>
@@ -3101,7 +3121,7 @@
       <c r="O32" s="10"/>
       <c r="P32" s="10"/>
     </row>
-    <row r="33" spans="1:16" s="11" customFormat="1" ht="13" thickTop="1">
+    <row r="33" spans="1:16" s="11" customFormat="1" ht="13.5" thickTop="1">
       <c r="A33" s="44" t="s">
         <v>45</v>
       </c>
@@ -3149,7 +3169,7 @@
       <c r="O34" s="10"/>
       <c r="P34" s="10"/>
     </row>
-    <row r="35" spans="1:16" s="11" customFormat="1" ht="24">
+    <row r="35" spans="1:16" s="11" customFormat="1" ht="25.5">
       <c r="A35" s="25" t="s">
         <v>44</v>
       </c>
@@ -3349,7 +3369,7 @@
       <c r="O44" s="2"/>
       <c r="P44" s="2"/>
     </row>
-    <row r="45" spans="1:16" s="4" customFormat="1" ht="15" hidden="1">
+    <row r="45" spans="1:16" s="4" customFormat="1" ht="15.75" hidden="1">
       <c r="A45" s="5" t="s">
         <v>2</v>
       </c>
@@ -3389,7 +3409,7 @@
       <c r="O46" s="2"/>
       <c r="P46" s="2"/>
     </row>
-    <row r="47" spans="1:16" s="4" customFormat="1" hidden="1">
+    <row r="47" spans="1:16" s="4" customFormat="1" ht="25.5" hidden="1">
       <c r="A47" s="6" t="s">
         <v>4</v>
       </c>
@@ -3502,7 +3522,7 @@
       <c r="O51" s="2"/>
       <c r="P51" s="2"/>
     </row>
-    <row r="53" spans="1:16" s="4" customFormat="1" ht="17" customHeight="1">
+    <row r="53" spans="1:16" s="4" customFormat="1" ht="17.100000000000001" customHeight="1">
       <c r="A53" s="15" t="s">
         <v>11</v>
       </c>
@@ -3550,20 +3570,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:P44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:C13"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="68.1640625" customWidth="1"/>
-    <col min="2" max="3" width="12.1640625" customWidth="1"/>
+    <col min="1" max="1" width="68.140625" customWidth="1"/>
+    <col min="2" max="3" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="4" customFormat="1" ht="15">
+    <row r="1" spans="1:16" s="4" customFormat="1" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3639,7 +3659,7 @@
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
     </row>
-    <row r="5" spans="1:16" s="4" customFormat="1" ht="15">
+    <row r="5" spans="1:16" s="4" customFormat="1" ht="15.75">
       <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
@@ -3695,7 +3715,7 @@
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
     </row>
-    <row r="8" spans="1:16" s="4" customFormat="1" ht="15">
+    <row r="8" spans="1:16" s="4" customFormat="1" ht="15.75">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -3735,7 +3755,7 @@
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
     </row>
-    <row r="10" spans="1:16" s="4" customFormat="1">
+    <row r="10" spans="1:16" s="4" customFormat="1" ht="25.5">
       <c r="A10" s="6" t="s">
         <v>4</v>
       </c>
@@ -3783,7 +3803,7 @@
       <c r="O11" s="10"/>
       <c r="P11" s="10"/>
     </row>
-    <row r="12" spans="1:16" s="11" customFormat="1" ht="13" thickBot="1">
+    <row r="12" spans="1:16" s="11" customFormat="1" ht="13.5" thickBot="1">
       <c r="A12" s="31" t="s">
         <v>51</v>
       </c>
@@ -3807,7 +3827,7 @@
       <c r="O12" s="10"/>
       <c r="P12" s="10"/>
     </row>
-    <row r="13" spans="1:16" s="11" customFormat="1" ht="25" thickTop="1">
+    <row r="13" spans="1:16" s="11" customFormat="1" ht="26.25" thickTop="1">
       <c r="A13" s="44" t="s">
         <v>53</v>
       </c>
@@ -3832,9 +3852,15 @@
       <c r="P13" s="10"/>
     </row>
     <row r="14" spans="1:16" s="11" customFormat="1">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="9"/>
+      <c r="A14" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" s="54">
+        <v>30</v>
+      </c>
+      <c r="C14" s="55">
+        <v>41629</v>
+      </c>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
@@ -3849,10 +3875,16 @@
       <c r="O14" s="10"/>
       <c r="P14" s="10"/>
     </row>
-    <row r="15" spans="1:16" s="11" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="12"/>
+    <row r="15" spans="1:16" s="11" customFormat="1">
+      <c r="A15" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="54">
+        <v>45</v>
+      </c>
+      <c r="C15" s="55">
+        <v>41630</v>
+      </c>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
@@ -3867,50 +3899,56 @@
       <c r="O15" s="10"/>
       <c r="P15" s="10"/>
     </row>
-    <row r="16" spans="1:16" s="4" customFormat="1">
-      <c r="A16" s="13" t="s">
+    <row r="16" spans="1:16" s="11" customFormat="1" ht="25.5">
+      <c r="A16" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" s="8">
+        <v>60</v>
+      </c>
+      <c r="C16" s="9">
+        <v>41630</v>
+      </c>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="10"/>
+    </row>
+    <row r="17" spans="1:16" s="11" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="10"/>
+    </row>
+    <row r="18" spans="1:16" s="4" customFormat="1">
+      <c r="A18" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="18">
-        <f>SUM(B11:B15)</f>
-        <v>170</v>
-      </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
-      <c r="P16" s="2"/>
-    </row>
-    <row r="17" spans="1:16" s="4" customFormat="1">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
-      <c r="P17" s="2"/>
-    </row>
-    <row r="18" spans="1:16" s="4" customFormat="1">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
+      <c r="B18" s="18">
+        <f>SUM(B11:B17)</f>
+        <v>305</v>
+      </c>
       <c r="C18" s="3"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -3944,14 +3982,10 @@
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
     </row>
-    <row r="20" spans="1:16" s="4" customFormat="1" ht="15">
-      <c r="A20" s="5" t="s">
-        <v>9</v>
-      </c>
+    <row r="20" spans="1:16" s="4" customFormat="1">
+      <c r="A20" s="2"/>
       <c r="B20" s="2"/>
-      <c r="C20" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="C20" s="3"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
@@ -3984,15 +4018,13 @@
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
     </row>
-    <row r="22" spans="1:16" s="4" customFormat="1">
-      <c r="A22" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>6</v>
+    <row r="22" spans="1:16" s="4" customFormat="1" ht="15.75">
+      <c r="A22" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -4008,63 +4040,57 @@
       <c r="O22" s="2"/>
       <c r="P22" s="2"/>
     </row>
-    <row r="23" spans="1:16" s="11" customFormat="1">
-      <c r="A23" s="23" t="s">
+    <row r="23" spans="1:16" s="4" customFormat="1">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+    </row>
+    <row r="24" spans="1:16" s="4" customFormat="1" ht="25.5">
+      <c r="A24" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+    </row>
+    <row r="25" spans="1:16" s="11" customFormat="1">
+      <c r="A25" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="B23" s="23">
+      <c r="B25" s="23">
         <v>60</v>
       </c>
-      <c r="C23" s="24" t="s">
+      <c r="C25" s="24" t="s">
         <v>38</v>
-      </c>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="10"/>
-      <c r="K23" s="10"/>
-      <c r="L23" s="10"/>
-      <c r="M23" s="10"/>
-      <c r="N23" s="10"/>
-      <c r="O23" s="10"/>
-      <c r="P23" s="10"/>
-    </row>
-    <row r="24" spans="1:16" s="11" customFormat="1" ht="13" thickBot="1">
-      <c r="A24" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="B24" s="31">
-        <v>35</v>
-      </c>
-      <c r="C24" s="32" t="s">
-        <v>38</v>
-      </c>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
-      <c r="K24" s="10"/>
-      <c r="L24" s="10"/>
-      <c r="M24" s="10"/>
-      <c r="N24" s="10"/>
-      <c r="O24" s="10"/>
-      <c r="P24" s="10"/>
-    </row>
-    <row r="25" spans="1:16" s="11" customFormat="1" ht="25" thickTop="1">
-      <c r="A25" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="B25" s="44">
-        <v>90</v>
-      </c>
-      <c r="C25" s="52" t="s">
-        <v>54</v>
       </c>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
@@ -4080,10 +4106,16 @@
       <c r="O25" s="10"/>
       <c r="P25" s="10"/>
     </row>
-    <row r="26" spans="1:16" s="11" customFormat="1">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="9"/>
+    <row r="26" spans="1:16" s="11" customFormat="1" ht="13.5" thickBot="1">
+      <c r="A26" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="31">
+        <v>35</v>
+      </c>
+      <c r="C26" s="32" t="s">
+        <v>38</v>
+      </c>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
@@ -4098,10 +4130,16 @@
       <c r="O26" s="10"/>
       <c r="P26" s="10"/>
     </row>
-    <row r="27" spans="1:16" s="11" customFormat="1">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="9"/>
+    <row r="27" spans="1:16" s="11" customFormat="1" ht="26.25" thickTop="1">
+      <c r="A27" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" s="44">
+        <v>90</v>
+      </c>
+      <c r="C27" s="52" t="s">
+        <v>54</v>
+      </c>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
@@ -4134,10 +4172,10 @@
       <c r="O28" s="10"/>
       <c r="P28" s="10"/>
     </row>
-    <row r="29" spans="1:16" s="11" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A29" s="10"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="12"/>
+    <row r="29" spans="1:16" s="11" customFormat="1">
+      <c r="A29" s="8"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="9"/>
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
       <c r="F29" s="10"/>
@@ -4152,50 +4190,56 @@
       <c r="O29" s="10"/>
       <c r="P29" s="10"/>
     </row>
-    <row r="30" spans="1:16" s="4" customFormat="1">
-      <c r="A30" s="13" t="s">
+    <row r="30" spans="1:16" s="11" customFormat="1" ht="25.5">
+      <c r="A30" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" s="23">
+        <v>60</v>
+      </c>
+      <c r="C30" s="24">
+        <v>41630</v>
+      </c>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="10"/>
+      <c r="M30" s="10"/>
+      <c r="N30" s="10"/>
+      <c r="O30" s="10"/>
+      <c r="P30" s="10"/>
+    </row>
+    <row r="31" spans="1:16" s="11" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A31" s="10"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
+      <c r="K31" s="10"/>
+      <c r="L31" s="10"/>
+      <c r="M31" s="10"/>
+      <c r="N31" s="10"/>
+      <c r="O31" s="10"/>
+      <c r="P31" s="10"/>
+    </row>
+    <row r="32" spans="1:16" s="4" customFormat="1">
+      <c r="A32" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B30" s="18">
-        <f>SUM(B23:B29)</f>
-        <v>185</v>
-      </c>
-      <c r="C30" s="3"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
-      <c r="L30" s="2"/>
-      <c r="M30" s="2"/>
-      <c r="N30" s="2"/>
-      <c r="O30" s="2"/>
-      <c r="P30" s="2"/>
-    </row>
-    <row r="31" spans="1:16" s="4" customFormat="1">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="2"/>
-      <c r="M31" s="2"/>
-      <c r="N31" s="2"/>
-      <c r="O31" s="2"/>
-      <c r="P31" s="2"/>
-    </row>
-    <row r="32" spans="1:16" s="4" customFormat="1" hidden="1">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
+      <c r="B32" s="18">
+        <f>SUM(B25:B31)</f>
+        <v>245</v>
+      </c>
       <c r="C32" s="3"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -4211,7 +4255,7 @@
       <c r="O32" s="2"/>
       <c r="P32" s="2"/>
     </row>
-    <row r="33" spans="1:16" s="4" customFormat="1" hidden="1">
+    <row r="33" spans="1:16" s="4" customFormat="1">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="3"/>
@@ -4229,14 +4273,10 @@
       <c r="O33" s="2"/>
       <c r="P33" s="2"/>
     </row>
-    <row r="34" spans="1:16" s="4" customFormat="1" ht="15" hidden="1">
-      <c r="A34" s="5" t="s">
-        <v>2</v>
-      </c>
+    <row r="34" spans="1:16" s="4" customFormat="1" hidden="1">
+      <c r="A34" s="2"/>
       <c r="B34" s="2"/>
-      <c r="C34" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="C34" s="3"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
@@ -4269,15 +4309,13 @@
       <c r="O35" s="2"/>
       <c r="P35" s="2"/>
     </row>
-    <row r="36" spans="1:16" s="4" customFormat="1" hidden="1">
-      <c r="A36" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>6</v>
+    <row r="36" spans="1:16" s="4" customFormat="1" ht="15.75" hidden="1">
+      <c r="A36" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B36" s="2"/>
+      <c r="C36" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -4293,58 +4331,58 @@
       <c r="O36" s="2"/>
       <c r="P36" s="2"/>
     </row>
-    <row r="37" spans="1:16" s="11" customFormat="1" ht="25.5" hidden="1" customHeight="1">
-      <c r="A37" s="8" t="s">
+    <row r="37" spans="1:16" s="4" customFormat="1" hidden="1">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+      <c r="O37" s="2"/>
+      <c r="P37" s="2"/>
+    </row>
+    <row r="38" spans="1:16" s="4" customFormat="1" ht="25.5" hidden="1">
+      <c r="A38" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
+      <c r="O38" s="2"/>
+      <c r="P38" s="2"/>
+    </row>
+    <row r="39" spans="1:16" s="11" customFormat="1" ht="25.5" hidden="1" customHeight="1">
+      <c r="A39" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B37" s="8">
+      <c r="B39" s="8">
         <v>0</v>
       </c>
-      <c r="C37" s="9">
+      <c r="C39" s="9">
         <v>41275</v>
       </c>
-      <c r="D37" s="10"/>
-      <c r="E37" s="10"/>
-      <c r="F37" s="10"/>
-      <c r="G37" s="10"/>
-      <c r="H37" s="10"/>
-      <c r="I37" s="10"/>
-      <c r="J37" s="10"/>
-      <c r="K37" s="10"/>
-      <c r="L37" s="10"/>
-      <c r="M37" s="10"/>
-      <c r="N37" s="10"/>
-      <c r="O37" s="10"/>
-      <c r="P37" s="10"/>
-    </row>
-    <row r="38" spans="1:16" s="11" customFormat="1" ht="25.5" hidden="1" customHeight="1">
-      <c r="A38" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B38" s="8">
-        <v>0</v>
-      </c>
-      <c r="C38" s="9">
-        <v>41275</v>
-      </c>
-      <c r="D38" s="10"/>
-      <c r="E38" s="10"/>
-      <c r="F38" s="10"/>
-      <c r="G38" s="10"/>
-      <c r="H38" s="10"/>
-      <c r="I38" s="10"/>
-      <c r="J38" s="10"/>
-      <c r="K38" s="10"/>
-      <c r="L38" s="10"/>
-      <c r="M38" s="10"/>
-      <c r="N38" s="10"/>
-      <c r="O38" s="10"/>
-      <c r="P38" s="10"/>
-    </row>
-    <row r="39" spans="1:16" s="11" customFormat="1" ht="12.75" hidden="1" customHeight="1">
-      <c r="A39" s="10"/>
-      <c r="B39" s="10"/>
-      <c r="C39" s="12"/>
       <c r="D39" s="10"/>
       <c r="E39" s="10"/>
       <c r="F39" s="10"/>
@@ -4359,41 +4397,57 @@
       <c r="O39" s="10"/>
       <c r="P39" s="10"/>
     </row>
-    <row r="40" spans="1:16" s="4" customFormat="1">
-      <c r="A40" s="13" t="s">
+    <row r="40" spans="1:16" s="11" customFormat="1" ht="25.5" hidden="1" customHeight="1">
+      <c r="A40" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="8">
+        <v>0</v>
+      </c>
+      <c r="C40" s="9">
+        <v>41275</v>
+      </c>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="10"/>
+      <c r="J40" s="10"/>
+      <c r="K40" s="10"/>
+      <c r="L40" s="10"/>
+      <c r="M40" s="10"/>
+      <c r="N40" s="10"/>
+      <c r="O40" s="10"/>
+      <c r="P40" s="10"/>
+    </row>
+    <row r="41" spans="1:16" s="11" customFormat="1" ht="12.75" hidden="1" customHeight="1">
+      <c r="A41" s="10"/>
+      <c r="B41" s="10"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10"/>
+      <c r="I41" s="10"/>
+      <c r="J41" s="10"/>
+      <c r="K41" s="10"/>
+      <c r="L41" s="10"/>
+      <c r="M41" s="10"/>
+      <c r="N41" s="10"/>
+      <c r="O41" s="10"/>
+      <c r="P41" s="10"/>
+    </row>
+    <row r="42" spans="1:16" s="4" customFormat="1">
+      <c r="A42" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B40" s="14">
-        <f>SUM(B37:B39)</f>
+      <c r="B42" s="14">
+        <f>SUM(B39:B41)</f>
         <v>0</v>
       </c>
-      <c r="C40" s="3"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
-      <c r="J40" s="2"/>
-      <c r="K40" s="2"/>
-      <c r="L40" s="2"/>
-      <c r="M40" s="2"/>
-      <c r="N40" s="2"/>
-      <c r="O40" s="2"/>
-      <c r="P40" s="2"/>
-    </row>
-    <row r="42" spans="1:16" s="4" customFormat="1" ht="17" customHeight="1">
-      <c r="A42" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B42" s="16">
-        <f>SUM(B30,B16)</f>
-        <v>355</v>
-      </c>
-      <c r="C42" s="17">
-        <f>TIME(0,B42,)</f>
-        <v>0.24652777777777779</v>
-      </c>
+      <c r="C42" s="3"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
@@ -4407,6 +4461,32 @@
       <c r="N42" s="2"/>
       <c r="O42" s="2"/>
       <c r="P42" s="2"/>
+    </row>
+    <row r="44" spans="1:16" s="4" customFormat="1" ht="17.100000000000001" customHeight="1">
+      <c r="A44" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B44" s="16">
+        <f>SUM(B32,B18)</f>
+        <v>550</v>
+      </c>
+      <c r="C44" s="17">
+        <f>TIME(0,B44,)</f>
+        <v>0.38194444444444442</v>
+      </c>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
+      <c r="O44" s="2"/>
+      <c r="P44" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Updated any document type and the lernjournal
</commit_message>
<xml_diff>
--- a/2_Semester/aufgabe_3+4+5_team_3_lernjournal.xlsx
+++ b/2_Semester/aufgabe_3+4+5_team_3_lernjournal.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="36735" yWindow="1515" windowWidth="20730" windowHeight="11760" tabRatio="415" activeTab="2"/>
+    <workbookView xWindow="42600" yWindow="880" windowWidth="27000" windowHeight="18780" tabRatio="415" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Lernjournal Aufgabe 3" sheetId="3" r:id="rId1"/>
     <sheet name="Lernjournal Aufgabe 4" sheetId="2" r:id="rId2"/>
     <sheet name="Lernjournal Aufgabe 5" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="64">
   <si>
     <t>Anleitung zum Lernjournal:</t>
   </si>
@@ -224,19 +224,31 @@
 Übernahme der Erkenntisse ins Klassendiagramm</t>
   </si>
   <si>
-    <t>Besprechung und Endversion Sequenzdiagramm. _x000D_
-Übernahme der Erkenntisse ins Klassendiagramm</t>
+    <t>Klassendiagramm für Business-Layer "fertig" gestellt. Viele offenen Fragen! Trotz  versuch in Eclipse zur Prüfung des Verständnisses. Aufgbanenteilung Sequenzdiagramm und Glossar.</t>
+  </si>
+  <si>
+    <t>21.12.13</t>
+  </si>
+  <si>
+    <t>22.12.13</t>
+  </si>
+  <si>
+    <t>Glossar V1 ergänzt um neue Interfaces und Klassen.</t>
+  </si>
+  <si>
+    <t>Glossar fertigstellen, minimale Korrekturen Diagramme und erstellung Bilder für Dokument.
+Erstellen des Dokuments für die Abgabe.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="???\ &quot;Minuten&quot;"/>
     <numFmt numFmtId="165" formatCode="[hh]:mm\ &quot;Std:Min&quot;"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -424,8 +436,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="129">
+  <cellStyleXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -713,145 +727,147 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="129">
-    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="92" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="94" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="96" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="98" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="100" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="102" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="104" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="106" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="108" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="110" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="112" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="114" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="116" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="118" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="120" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="122" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="124" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="126" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="128" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+  <cellStyles count="131">
+    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="129" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1180,20 +1196,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P57"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="68.140625" customWidth="1"/>
-    <col min="2" max="3" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="68.1640625" customWidth="1"/>
+    <col min="2" max="3" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="4" customFormat="1" ht="15.75">
+    <row r="1" spans="1:16" s="4" customFormat="1" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1214,11 +1230,11 @@
       <c r="P1" s="2"/>
     </row>
     <row r="2" spans="1:16" s="4" customFormat="1" ht="60" customHeight="1">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -1269,7 +1285,7 @@
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
     </row>
-    <row r="5" spans="1:16" s="4" customFormat="1" ht="15.75">
+    <row r="5" spans="1:16" s="4" customFormat="1" ht="15">
       <c r="A5" s="5" t="s">
         <v>13</v>
       </c>
@@ -1325,7 +1341,7 @@
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
     </row>
-    <row r="8" spans="1:16" s="4" customFormat="1" ht="15.75">
+    <row r="8" spans="1:16" s="4" customFormat="1" ht="15">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -1365,7 +1381,7 @@
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
     </row>
-    <row r="10" spans="1:16" s="4" customFormat="1" ht="25.5">
+    <row r="10" spans="1:16" s="4" customFormat="1">
       <c r="A10" s="6" t="s">
         <v>4</v>
       </c>
@@ -1485,7 +1501,7 @@
       <c r="O14" s="10"/>
       <c r="P14" s="10"/>
     </row>
-    <row r="15" spans="1:16" s="11" customFormat="1" ht="39" thickBot="1">
+    <row r="15" spans="1:16" s="11" customFormat="1" ht="37" thickBot="1">
       <c r="A15" s="30" t="s">
         <v>19</v>
       </c>
@@ -1509,7 +1525,7 @@
       <c r="O15" s="10"/>
       <c r="P15" s="10"/>
     </row>
-    <row r="16" spans="1:16" s="11" customFormat="1" ht="13.5" thickTop="1">
+    <row r="16" spans="1:16" s="11" customFormat="1" ht="13" thickTop="1">
       <c r="A16" s="33" t="s">
         <v>24</v>
       </c>
@@ -1581,7 +1597,7 @@
       <c r="O18" s="10"/>
       <c r="P18" s="10"/>
     </row>
-    <row r="19" spans="1:16" s="11" customFormat="1" ht="26.25" thickBot="1">
+    <row r="19" spans="1:16" s="11" customFormat="1" ht="25" thickBot="1">
       <c r="A19" s="36" t="s">
         <v>28</v>
       </c>
@@ -1605,7 +1621,7 @@
       <c r="O19" s="10"/>
       <c r="P19" s="10"/>
     </row>
-    <row r="20" spans="1:16" s="11" customFormat="1" ht="13.5" thickTop="1">
+    <row r="20" spans="1:16" s="11" customFormat="1" ht="13" thickTop="1">
       <c r="A20" s="39" t="s">
         <v>29</v>
       </c>
@@ -1769,7 +1785,7 @@
       <c r="O27" s="2"/>
       <c r="P27" s="2"/>
     </row>
-    <row r="28" spans="1:16" s="4" customFormat="1" ht="15.75">
+    <row r="28" spans="1:16" s="4" customFormat="1" ht="15">
       <c r="A28" s="5" t="s">
         <v>9</v>
       </c>
@@ -1809,7 +1825,7 @@
       <c r="O29" s="2"/>
       <c r="P29" s="2"/>
     </row>
-    <row r="30" spans="1:16" s="4" customFormat="1" ht="25.5">
+    <row r="30" spans="1:16" s="4" customFormat="1">
       <c r="A30" s="6" t="s">
         <v>4</v>
       </c>
@@ -1833,7 +1849,7 @@
       <c r="O30" s="2"/>
       <c r="P30" s="2"/>
     </row>
-    <row r="31" spans="1:16" s="11" customFormat="1" ht="25.5">
+    <row r="31" spans="1:16" s="11" customFormat="1">
       <c r="A31" s="29" t="s">
         <v>20</v>
       </c>
@@ -1881,7 +1897,7 @@
       <c r="O32" s="10"/>
       <c r="P32" s="10"/>
     </row>
-    <row r="33" spans="1:16" s="11" customFormat="1" ht="25.5">
+    <row r="33" spans="1:16" s="11" customFormat="1">
       <c r="A33" s="23" t="s">
         <v>22</v>
       </c>
@@ -1929,7 +1945,7 @@
       <c r="O34" s="10"/>
       <c r="P34" s="10"/>
     </row>
-    <row r="35" spans="1:16" s="11" customFormat="1" ht="39" thickBot="1">
+    <row r="35" spans="1:16" s="11" customFormat="1" ht="37" thickBot="1">
       <c r="A35" s="30" t="s">
         <v>19</v>
       </c>
@@ -1953,7 +1969,7 @@
       <c r="O35" s="10"/>
       <c r="P35" s="10"/>
     </row>
-    <row r="36" spans="1:16" s="11" customFormat="1" ht="39" thickTop="1">
+    <row r="36" spans="1:16" s="11" customFormat="1" ht="25" thickTop="1">
       <c r="A36" s="33" t="s">
         <v>14</v>
       </c>
@@ -2073,7 +2089,7 @@
       <c r="O40" s="10"/>
       <c r="P40" s="10"/>
     </row>
-    <row r="41" spans="1:16" s="11" customFormat="1" ht="26.25" thickBot="1">
+    <row r="41" spans="1:16" s="11" customFormat="1" ht="25" thickBot="1">
       <c r="A41" s="36" t="s">
         <v>28</v>
       </c>
@@ -2097,7 +2113,7 @@
       <c r="O41" s="10"/>
       <c r="P41" s="10"/>
     </row>
-    <row r="42" spans="1:16" s="11" customFormat="1" ht="13.5" thickTop="1">
+    <row r="42" spans="1:16" s="11" customFormat="1" ht="13" thickTop="1">
       <c r="A42" s="25" t="s">
         <v>30</v>
       </c>
@@ -2243,7 +2259,7 @@
       <c r="O48" s="2"/>
       <c r="P48" s="2"/>
     </row>
-    <row r="49" spans="1:16" s="4" customFormat="1" ht="15.75" hidden="1">
+    <row r="49" spans="1:16" s="4" customFormat="1" ht="15" hidden="1">
       <c r="A49" s="5" t="s">
         <v>2</v>
       </c>
@@ -2283,7 +2299,7 @@
       <c r="O50" s="2"/>
       <c r="P50" s="2"/>
     </row>
-    <row r="51" spans="1:16" s="4" customFormat="1" ht="25.5" hidden="1">
+    <row r="51" spans="1:16" s="4" customFormat="1" hidden="1">
       <c r="A51" s="6" t="s">
         <v>4</v>
       </c>
@@ -2396,7 +2412,7 @@
       <c r="O55" s="2"/>
       <c r="P55" s="2"/>
     </row>
-    <row r="57" spans="1:16" s="4" customFormat="1" ht="17.100000000000001" customHeight="1">
+    <row r="57" spans="1:16" s="4" customFormat="1" ht="17" customHeight="1">
       <c r="A57" s="15" t="s">
         <v>11</v>
       </c>
@@ -2444,20 +2460,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P53"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="68.140625" customWidth="1"/>
-    <col min="2" max="3" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="68.1640625" customWidth="1"/>
+    <col min="2" max="3" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="4" customFormat="1" ht="15.75">
+    <row r="1" spans="1:16" s="4" customFormat="1" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2478,11 +2494,11 @@
       <c r="P1" s="2"/>
     </row>
     <row r="2" spans="1:16" s="4" customFormat="1" ht="60" customHeight="1">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -2533,7 +2549,7 @@
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
     </row>
-    <row r="5" spans="1:16" s="4" customFormat="1" ht="15.75">
+    <row r="5" spans="1:16" s="4" customFormat="1" ht="15">
       <c r="A5" s="5" t="s">
         <v>13</v>
       </c>
@@ -2589,7 +2605,7 @@
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
     </row>
-    <row r="8" spans="1:16" s="4" customFormat="1" ht="15.75">
+    <row r="8" spans="1:16" s="4" customFormat="1" ht="15">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -2629,7 +2645,7 @@
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
     </row>
-    <row r="10" spans="1:16" s="4" customFormat="1" ht="25.5">
+    <row r="10" spans="1:16" s="4" customFormat="1">
       <c r="A10" s="6" t="s">
         <v>4</v>
       </c>
@@ -2677,7 +2693,7 @@
       <c r="O11" s="10"/>
       <c r="P11" s="10"/>
     </row>
-    <row r="12" spans="1:16" s="11" customFormat="1" ht="13.5" thickBot="1">
+    <row r="12" spans="1:16" s="11" customFormat="1" ht="13" thickBot="1">
       <c r="A12" s="30" t="s">
         <v>39</v>
       </c>
@@ -2701,7 +2717,7 @@
       <c r="O12" s="10"/>
       <c r="P12" s="10"/>
     </row>
-    <row r="13" spans="1:16" s="11" customFormat="1" ht="13.5" thickTop="1">
+    <row r="13" spans="1:16" s="11" customFormat="1" ht="13" thickTop="1">
       <c r="A13" s="44"/>
       <c r="B13" s="34"/>
       <c r="C13" s="35"/>
@@ -2719,7 +2735,7 @@
       <c r="O13" s="10"/>
       <c r="P13" s="10"/>
     </row>
-    <row r="14" spans="1:16" s="11" customFormat="1" ht="25.5">
+    <row r="14" spans="1:16" s="11" customFormat="1" ht="24">
       <c r="A14" s="20" t="s">
         <v>44</v>
       </c>
@@ -2743,7 +2759,7 @@
       <c r="O14" s="10"/>
       <c r="P14" s="10"/>
     </row>
-    <row r="15" spans="1:16" s="11" customFormat="1" ht="25.5">
+    <row r="15" spans="1:16" s="11" customFormat="1" ht="24">
       <c r="A15" s="25" t="s">
         <v>49</v>
       </c>
@@ -2937,7 +2953,7 @@
       <c r="O24" s="2"/>
       <c r="P24" s="2"/>
     </row>
-    <row r="25" spans="1:16" s="4" customFormat="1" ht="15.75">
+    <row r="25" spans="1:16" s="4" customFormat="1" ht="15">
       <c r="A25" s="5" t="s">
         <v>9</v>
       </c>
@@ -2977,7 +2993,7 @@
       <c r="O26" s="2"/>
       <c r="P26" s="2"/>
     </row>
-    <row r="27" spans="1:16" s="4" customFormat="1" ht="25.5">
+    <row r="27" spans="1:16" s="4" customFormat="1">
       <c r="A27" s="6" t="s">
         <v>4</v>
       </c>
@@ -3025,7 +3041,7 @@
       <c r="O28" s="10"/>
       <c r="P28" s="10"/>
     </row>
-    <row r="29" spans="1:16" s="11" customFormat="1" ht="25.5">
+    <row r="29" spans="1:16" s="11" customFormat="1" ht="24">
       <c r="A29" s="23" t="s">
         <v>33</v>
       </c>
@@ -3097,7 +3113,7 @@
       <c r="O31" s="10"/>
       <c r="P31" s="10"/>
     </row>
-    <row r="32" spans="1:16" s="11" customFormat="1" ht="13.5" thickBot="1">
+    <row r="32" spans="1:16" s="11" customFormat="1" ht="13" thickBot="1">
       <c r="A32" s="30" t="s">
         <v>39</v>
       </c>
@@ -3121,7 +3137,7 @@
       <c r="O32" s="10"/>
       <c r="P32" s="10"/>
     </row>
-    <row r="33" spans="1:16" s="11" customFormat="1" ht="13.5" thickTop="1">
+    <row r="33" spans="1:16" s="11" customFormat="1" ht="13" thickTop="1">
       <c r="A33" s="44" t="s">
         <v>45</v>
       </c>
@@ -3169,7 +3185,7 @@
       <c r="O34" s="10"/>
       <c r="P34" s="10"/>
     </row>
-    <row r="35" spans="1:16" s="11" customFormat="1" ht="25.5">
+    <row r="35" spans="1:16" s="11" customFormat="1" ht="24">
       <c r="A35" s="25" t="s">
         <v>44</v>
       </c>
@@ -3369,7 +3385,7 @@
       <c r="O44" s="2"/>
       <c r="P44" s="2"/>
     </row>
-    <row r="45" spans="1:16" s="4" customFormat="1" ht="15.75" hidden="1">
+    <row r="45" spans="1:16" s="4" customFormat="1" ht="15" hidden="1">
       <c r="A45" s="5" t="s">
         <v>2</v>
       </c>
@@ -3409,7 +3425,7 @@
       <c r="O46" s="2"/>
       <c r="P46" s="2"/>
     </row>
-    <row r="47" spans="1:16" s="4" customFormat="1" ht="25.5" hidden="1">
+    <row r="47" spans="1:16" s="4" customFormat="1" hidden="1">
       <c r="A47" s="6" t="s">
         <v>4</v>
       </c>
@@ -3522,7 +3538,7 @@
       <c r="O51" s="2"/>
       <c r="P51" s="2"/>
     </row>
-    <row r="53" spans="1:16" s="4" customFormat="1" ht="17.100000000000001" customHeight="1">
+    <row r="53" spans="1:16" s="4" customFormat="1" ht="17" customHeight="1">
       <c r="A53" s="15" t="s">
         <v>11</v>
       </c>
@@ -3570,20 +3586,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="68.140625" customWidth="1"/>
-    <col min="2" max="3" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="68.1640625" customWidth="1"/>
+    <col min="2" max="3" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="4" customFormat="1" ht="15.75">
+    <row r="1" spans="1:16" s="4" customFormat="1" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3604,11 +3620,11 @@
       <c r="P1" s="2"/>
     </row>
     <row r="2" spans="1:16" s="4" customFormat="1" ht="60" customHeight="1">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -3659,7 +3675,7 @@
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
     </row>
-    <row r="5" spans="1:16" s="4" customFormat="1" ht="15.75">
+    <row r="5" spans="1:16" s="4" customFormat="1" ht="15">
       <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
@@ -3715,7 +3731,7 @@
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
     </row>
-    <row r="8" spans="1:16" s="4" customFormat="1" ht="15.75">
+    <row r="8" spans="1:16" s="4" customFormat="1" ht="15">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -3755,7 +3771,7 @@
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
     </row>
-    <row r="10" spans="1:16" s="4" customFormat="1" ht="25.5">
+    <row r="10" spans="1:16" s="4" customFormat="1">
       <c r="A10" s="6" t="s">
         <v>4</v>
       </c>
@@ -3803,7 +3819,7 @@
       <c r="O11" s="10"/>
       <c r="P11" s="10"/>
     </row>
-    <row r="12" spans="1:16" s="11" customFormat="1" ht="13.5" thickBot="1">
+    <row r="12" spans="1:16" s="11" customFormat="1" ht="13" thickBot="1">
       <c r="A12" s="31" t="s">
         <v>51</v>
       </c>
@@ -3827,7 +3843,7 @@
       <c r="O12" s="10"/>
       <c r="P12" s="10"/>
     </row>
-    <row r="13" spans="1:16" s="11" customFormat="1" ht="26.25" thickTop="1">
+    <row r="13" spans="1:16" s="11" customFormat="1" ht="25" thickTop="1">
       <c r="A13" s="44" t="s">
         <v>53</v>
       </c>
@@ -3851,15 +3867,15 @@
       <c r="O13" s="10"/>
       <c r="P13" s="10"/>
     </row>
-    <row r="14" spans="1:16" s="11" customFormat="1">
-      <c r="A14" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="B14" s="54">
-        <v>30</v>
-      </c>
-      <c r="C14" s="55">
-        <v>41629</v>
+    <row r="14" spans="1:16" s="11" customFormat="1" ht="36">
+      <c r="A14" s="53" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="53">
+        <v>150</v>
+      </c>
+      <c r="C14" s="54" t="s">
+        <v>60</v>
       </c>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
@@ -3877,13 +3893,13 @@
     </row>
     <row r="15" spans="1:16" s="11" customFormat="1">
       <c r="A15" s="39" t="s">
-        <v>56</v>
-      </c>
-      <c r="B15" s="54">
-        <v>45</v>
-      </c>
-      <c r="C15" s="55">
-        <v>41630</v>
+        <v>57</v>
+      </c>
+      <c r="B15" s="53">
+        <v>30</v>
+      </c>
+      <c r="C15" s="54" t="s">
+        <v>60</v>
       </c>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
@@ -3899,15 +3915,15 @@
       <c r="O15" s="10"/>
       <c r="P15" s="10"/>
     </row>
-    <row r="16" spans="1:16" s="11" customFormat="1" ht="25.5">
-      <c r="A16" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="B16" s="8">
-        <v>60</v>
-      </c>
-      <c r="C16" s="9">
-        <v>41630</v>
+    <row r="16" spans="1:16" s="11" customFormat="1">
+      <c r="A16" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="53">
+        <v>45</v>
+      </c>
+      <c r="C16" s="54" t="s">
+        <v>61</v>
       </c>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
@@ -3923,10 +3939,16 @@
       <c r="O16" s="10"/>
       <c r="P16" s="10"/>
     </row>
-    <row r="17" spans="1:16" s="11" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A17" s="10"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="12"/>
+    <row r="17" spans="1:16" s="11" customFormat="1" ht="24">
+      <c r="A17" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" s="8">
+        <v>60</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>61</v>
+      </c>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
@@ -3941,32 +3963,32 @@
       <c r="O17" s="10"/>
       <c r="P17" s="10"/>
     </row>
-    <row r="18" spans="1:16" s="4" customFormat="1">
-      <c r="A18" s="13" t="s">
+    <row r="18" spans="1:16" s="11" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="10"/>
+    </row>
+    <row r="19" spans="1:16" s="4" customFormat="1">
+      <c r="A19" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="18">
-        <f>SUM(B11:B17)</f>
-        <v>305</v>
-      </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
-      <c r="P18" s="2"/>
-    </row>
-    <row r="19" spans="1:16" s="4" customFormat="1">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
+      <c r="B19" s="18">
+        <f>SUM(B11:B18)</f>
+        <v>455</v>
+      </c>
       <c r="C19" s="3"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -4018,14 +4040,10 @@
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
     </row>
-    <row r="22" spans="1:16" s="4" customFormat="1" ht="15.75">
-      <c r="A22" s="5" t="s">
-        <v>9</v>
-      </c>
+    <row r="22" spans="1:16" s="4" customFormat="1">
+      <c r="A22" s="2"/>
       <c r="B22" s="2"/>
-      <c r="C22" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="C22" s="3"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
@@ -4040,10 +4058,14 @@
       <c r="O22" s="2"/>
       <c r="P22" s="2"/>
     </row>
-    <row r="23" spans="1:16" s="4" customFormat="1">
-      <c r="A23" s="2"/>
+    <row r="23" spans="1:16" s="4" customFormat="1" ht="15">
+      <c r="A23" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="B23" s="2"/>
-      <c r="C23" s="3"/>
+      <c r="C23" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
@@ -4058,16 +4080,10 @@
       <c r="O23" s="2"/>
       <c r="P23" s="2"/>
     </row>
-    <row r="24" spans="1:16" s="4" customFormat="1" ht="25.5">
-      <c r="A24" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>6</v>
-      </c>
+    <row r="24" spans="1:16" s="4" customFormat="1">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="3"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
@@ -4082,38 +4098,38 @@
       <c r="O24" s="2"/>
       <c r="P24" s="2"/>
     </row>
-    <row r="25" spans="1:16" s="11" customFormat="1">
-      <c r="A25" s="23" t="s">
+    <row r="25" spans="1:16" s="4" customFormat="1">
+      <c r="A25" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+    </row>
+    <row r="26" spans="1:16" s="11" customFormat="1">
+      <c r="A26" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="B25" s="23">
+      <c r="B26" s="23">
         <v>60</v>
       </c>
-      <c r="C25" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="10"/>
-      <c r="K25" s="10"/>
-      <c r="L25" s="10"/>
-      <c r="M25" s="10"/>
-      <c r="N25" s="10"/>
-      <c r="O25" s="10"/>
-      <c r="P25" s="10"/>
-    </row>
-    <row r="26" spans="1:16" s="11" customFormat="1" ht="13.5" thickBot="1">
-      <c r="A26" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="B26" s="31">
-        <v>35</v>
-      </c>
-      <c r="C26" s="32" t="s">
+      <c r="C26" s="24" t="s">
         <v>38</v>
       </c>
       <c r="D26" s="10"/>
@@ -4130,15 +4146,15 @@
       <c r="O26" s="10"/>
       <c r="P26" s="10"/>
     </row>
-    <row r="27" spans="1:16" s="11" customFormat="1" ht="26.25" thickTop="1">
-      <c r="A27" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="B27" s="44">
-        <v>90</v>
-      </c>
-      <c r="C27" s="52" t="s">
-        <v>54</v>
+    <row r="27" spans="1:16" s="11" customFormat="1" ht="13" thickBot="1">
+      <c r="A27" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" s="31">
+        <v>35</v>
+      </c>
+      <c r="C27" s="32" t="s">
+        <v>38</v>
       </c>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
@@ -4154,10 +4170,16 @@
       <c r="O27" s="10"/>
       <c r="P27" s="10"/>
     </row>
-    <row r="28" spans="1:16" s="11" customFormat="1">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="9"/>
+    <row r="28" spans="1:16" s="11" customFormat="1" ht="25" thickTop="1">
+      <c r="A28" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="44">
+        <v>90</v>
+      </c>
+      <c r="C28" s="52" t="s">
+        <v>54</v>
+      </c>
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
@@ -4172,10 +4194,16 @@
       <c r="O28" s="10"/>
       <c r="P28" s="10"/>
     </row>
-    <row r="29" spans="1:16" s="11" customFormat="1">
-      <c r="A29" s="8"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="9"/>
+    <row r="29" spans="1:16" s="11" customFormat="1" ht="36">
+      <c r="A29" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="B29" s="23">
+        <v>150</v>
+      </c>
+      <c r="C29" s="24" t="s">
+        <v>60</v>
+      </c>
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
       <c r="F29" s="10"/>
@@ -4190,15 +4218,15 @@
       <c r="O29" s="10"/>
       <c r="P29" s="10"/>
     </row>
-    <row r="30" spans="1:16" s="11" customFormat="1" ht="25.5">
-      <c r="A30" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="B30" s="23">
-        <v>60</v>
-      </c>
-      <c r="C30" s="24">
-        <v>41630</v>
+    <row r="30" spans="1:16" s="11" customFormat="1">
+      <c r="A30" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" s="8">
+        <v>30</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>61</v>
       </c>
       <c r="D30" s="10"/>
       <c r="E30" s="10"/>
@@ -4214,10 +4242,16 @@
       <c r="O30" s="10"/>
       <c r="P30" s="10"/>
     </row>
-    <row r="31" spans="1:16" s="11" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A31" s="10"/>
-      <c r="B31" s="10"/>
-      <c r="C31" s="12"/>
+    <row r="31" spans="1:16" s="11" customFormat="1" ht="24">
+      <c r="A31" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" s="23">
+        <v>60</v>
+      </c>
+      <c r="C31" s="24" t="s">
+        <v>61</v>
+      </c>
       <c r="D31" s="10"/>
       <c r="E31" s="10"/>
       <c r="F31" s="10"/>
@@ -4232,50 +4266,56 @@
       <c r="O31" s="10"/>
       <c r="P31" s="10"/>
     </row>
-    <row r="32" spans="1:16" s="4" customFormat="1">
-      <c r="A32" s="13" t="s">
+    <row r="32" spans="1:16" s="11" customFormat="1" ht="36">
+      <c r="A32" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B32" s="23">
+        <v>80</v>
+      </c>
+      <c r="C32" s="24">
+        <v>41631</v>
+      </c>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="10"/>
+      <c r="K32" s="10"/>
+      <c r="L32" s="10"/>
+      <c r="M32" s="10"/>
+      <c r="N32" s="10"/>
+      <c r="O32" s="10"/>
+      <c r="P32" s="10"/>
+    </row>
+    <row r="33" spans="1:16" s="11" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A33" s="10"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="10"/>
+      <c r="L33" s="10"/>
+      <c r="M33" s="10"/>
+      <c r="N33" s="10"/>
+      <c r="O33" s="10"/>
+      <c r="P33" s="10"/>
+    </row>
+    <row r="34" spans="1:16" s="4" customFormat="1">
+      <c r="A34" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B32" s="18">
-        <f>SUM(B25:B31)</f>
-        <v>245</v>
-      </c>
-      <c r="C32" s="3"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
-      <c r="L32" s="2"/>
-      <c r="M32" s="2"/>
-      <c r="N32" s="2"/>
-      <c r="O32" s="2"/>
-      <c r="P32" s="2"/>
-    </row>
-    <row r="33" spans="1:16" s="4" customFormat="1">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
-      <c r="L33" s="2"/>
-      <c r="M33" s="2"/>
-      <c r="N33" s="2"/>
-      <c r="O33" s="2"/>
-      <c r="P33" s="2"/>
-    </row>
-    <row r="34" spans="1:16" s="4" customFormat="1" hidden="1">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
+      <c r="B34" s="18">
+        <f>SUM(B26:B33)</f>
+        <v>505</v>
+      </c>
       <c r="C34" s="3"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
@@ -4291,7 +4331,7 @@
       <c r="O34" s="2"/>
       <c r="P34" s="2"/>
     </row>
-    <row r="35" spans="1:16" s="4" customFormat="1" hidden="1">
+    <row r="35" spans="1:16" s="4" customFormat="1">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="3"/>
@@ -4309,14 +4349,10 @@
       <c r="O35" s="2"/>
       <c r="P35" s="2"/>
     </row>
-    <row r="36" spans="1:16" s="4" customFormat="1" ht="15.75" hidden="1">
-      <c r="A36" s="5" t="s">
-        <v>2</v>
-      </c>
+    <row r="36" spans="1:16" s="4" customFormat="1" hidden="1">
+      <c r="A36" s="2"/>
       <c r="B36" s="2"/>
-      <c r="C36" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="C36" s="3"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
@@ -4349,15 +4385,13 @@
       <c r="O37" s="2"/>
       <c r="P37" s="2"/>
     </row>
-    <row r="38" spans="1:16" s="4" customFormat="1" ht="25.5" hidden="1">
-      <c r="A38" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C38" s="7" t="s">
-        <v>6</v>
+    <row r="38" spans="1:16" s="4" customFormat="1" ht="15" hidden="1">
+      <c r="A38" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B38" s="2"/>
+      <c r="C38" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
@@ -4373,58 +4407,58 @@
       <c r="O38" s="2"/>
       <c r="P38" s="2"/>
     </row>
-    <row r="39" spans="1:16" s="11" customFormat="1" ht="25.5" hidden="1" customHeight="1">
-      <c r="A39" s="8" t="s">
+    <row r="39" spans="1:16" s="4" customFormat="1" hidden="1">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
+      <c r="O39" s="2"/>
+      <c r="P39" s="2"/>
+    </row>
+    <row r="40" spans="1:16" s="4" customFormat="1" hidden="1">
+      <c r="A40" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
+      <c r="O40" s="2"/>
+      <c r="P40" s="2"/>
+    </row>
+    <row r="41" spans="1:16" s="11" customFormat="1" ht="25.5" hidden="1" customHeight="1">
+      <c r="A41" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B39" s="8">
+      <c r="B41" s="8">
         <v>0</v>
       </c>
-      <c r="C39" s="9">
+      <c r="C41" s="9">
         <v>41275</v>
       </c>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="10"/>
-      <c r="G39" s="10"/>
-      <c r="H39" s="10"/>
-      <c r="I39" s="10"/>
-      <c r="J39" s="10"/>
-      <c r="K39" s="10"/>
-      <c r="L39" s="10"/>
-      <c r="M39" s="10"/>
-      <c r="N39" s="10"/>
-      <c r="O39" s="10"/>
-      <c r="P39" s="10"/>
-    </row>
-    <row r="40" spans="1:16" s="11" customFormat="1" ht="25.5" hidden="1" customHeight="1">
-      <c r="A40" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B40" s="8">
-        <v>0</v>
-      </c>
-      <c r="C40" s="9">
-        <v>41275</v>
-      </c>
-      <c r="D40" s="10"/>
-      <c r="E40" s="10"/>
-      <c r="F40" s="10"/>
-      <c r="G40" s="10"/>
-      <c r="H40" s="10"/>
-      <c r="I40" s="10"/>
-      <c r="J40" s="10"/>
-      <c r="K40" s="10"/>
-      <c r="L40" s="10"/>
-      <c r="M40" s="10"/>
-      <c r="N40" s="10"/>
-      <c r="O40" s="10"/>
-      <c r="P40" s="10"/>
-    </row>
-    <row r="41" spans="1:16" s="11" customFormat="1" ht="12.75" hidden="1" customHeight="1">
-      <c r="A41" s="10"/>
-      <c r="B41" s="10"/>
-      <c r="C41" s="12"/>
       <c r="D41" s="10"/>
       <c r="E41" s="10"/>
       <c r="F41" s="10"/>
@@ -4439,41 +4473,57 @@
       <c r="O41" s="10"/>
       <c r="P41" s="10"/>
     </row>
-    <row r="42" spans="1:16" s="4" customFormat="1">
-      <c r="A42" s="13" t="s">
+    <row r="42" spans="1:16" s="11" customFormat="1" ht="25.5" hidden="1" customHeight="1">
+      <c r="A42" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" s="8">
+        <v>0</v>
+      </c>
+      <c r="C42" s="9">
+        <v>41275</v>
+      </c>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
+      <c r="H42" s="10"/>
+      <c r="I42" s="10"/>
+      <c r="J42" s="10"/>
+      <c r="K42" s="10"/>
+      <c r="L42" s="10"/>
+      <c r="M42" s="10"/>
+      <c r="N42" s="10"/>
+      <c r="O42" s="10"/>
+      <c r="P42" s="10"/>
+    </row>
+    <row r="43" spans="1:16" s="11" customFormat="1" ht="12.75" hidden="1" customHeight="1">
+      <c r="A43" s="10"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
+      <c r="H43" s="10"/>
+      <c r="I43" s="10"/>
+      <c r="J43" s="10"/>
+      <c r="K43" s="10"/>
+      <c r="L43" s="10"/>
+      <c r="M43" s="10"/>
+      <c r="N43" s="10"/>
+      <c r="O43" s="10"/>
+      <c r="P43" s="10"/>
+    </row>
+    <row r="44" spans="1:16" s="4" customFormat="1" hidden="1">
+      <c r="A44" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B42" s="14">
-        <f>SUM(B39:B41)</f>
+      <c r="B44" s="14">
+        <f>SUM(B41:B43)</f>
         <v>0</v>
       </c>
-      <c r="C42" s="3"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
-      <c r="K42" s="2"/>
-      <c r="L42" s="2"/>
-      <c r="M42" s="2"/>
-      <c r="N42" s="2"/>
-      <c r="O42" s="2"/>
-      <c r="P42" s="2"/>
-    </row>
-    <row r="44" spans="1:16" s="4" customFormat="1" ht="17.100000000000001" customHeight="1">
-      <c r="A44" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B44" s="16">
-        <f>SUM(B32,B18)</f>
-        <v>550</v>
-      </c>
-      <c r="C44" s="17">
-        <f>TIME(0,B44,)</f>
-        <v>0.38194444444444442</v>
-      </c>
+      <c r="C44" s="3"/>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
@@ -4487,6 +4537,32 @@
       <c r="N44" s="2"/>
       <c r="O44" s="2"/>
       <c r="P44" s="2"/>
+    </row>
+    <row r="46" spans="1:16" s="4" customFormat="1" ht="17" customHeight="1">
+      <c r="A46" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B46" s="16">
+        <f>SUM(B34,B19)</f>
+        <v>960</v>
+      </c>
+      <c r="C46" s="17">
+        <f>TIME(0,B46,)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+      <c r="L46" s="2"/>
+      <c r="M46" s="2"/>
+      <c r="N46" s="2"/>
+      <c r="O46" s="2"/>
+      <c r="P46" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>